<commit_message>
added changes to scrap all social media
</commit_message>
<xml_diff>
--- a/Albania.xlsx
+++ b/Albania.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,37 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>WebAddress</t>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Facebook Link</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Instagram Link</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Twitter Link</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>YouTube Link</t>
         </is>
       </c>
     </row>
@@ -469,6 +499,36 @@
           <t>https://pastadiamond.com/</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>+355684095232</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>info@agroblend.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/diamondpasta</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/pastadiamond/</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/channel/UCyuGDc-zc4j4NmXqLvXQR7g</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -487,6 +547,36 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>https://www.kraco.al/</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>+355 692070014</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>info@kraco.al</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/KracoAL</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/kraco_nature/</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/channel/UCLVWuZp1esG6f4ui66vKWdg</t>
         </is>
       </c>
     </row>

</xml_diff>